<commit_message>
Update layout and replace vid for img
</commit_message>
<xml_diff>
--- a/src/main/webapp/assets/movies.xlsx
+++ b/src/main/webapp/assets/movies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whitneykugel/CVTC Courses/JavaWebProgramming/Submitted/Movies_wkugel1/src/main/webapp/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whitneykugel/Coding/WhitneyKugel.com/BucketListMovies/src/main/webapp/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519D0117-85B0-824B-B2D8-CCF56DDB58E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB3FA08-2D91-964E-A41B-1D9A0177E718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50040" yWindow="-10300" windowWidth="29580" windowHeight="27420" xr2:uid="{E38C7BD9-DD28-C34F-B070-6A44E8CC0118}"/>
+    <workbookView xWindow="50040" yWindow="-6300" windowWidth="29580" windowHeight="27400" xr2:uid="{E38C7BD9-DD28-C34F-B070-6A44E8CC0118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,9 +578,6 @@
     <t>sY1S34973zA</t>
   </si>
   <si>
-    <t>EXeTwQWrcwY</t>
-  </si>
-  <si>
     <t>9O1Iy9od7-A</t>
   </si>
   <si>
@@ -720,6 +717,9 @@
   </si>
   <si>
     <t>dfeUzm6KF4g</t>
+  </si>
+  <si>
+    <t>DarkKnight.jpg</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1123,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1161,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1213,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1239,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1291,7 +1291,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1343,7 +1343,7 @@
         <v>43</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1369,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1395,7 +1395,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1421,7 +1421,7 @@
         <v>12</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="91" x14ac:dyDescent="0.2">
@@ -1447,7 +1447,7 @@
         <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1473,7 +1473,7 @@
         <v>27</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1499,7 +1499,7 @@
         <v>12</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1525,7 +1525,7 @@
         <v>64</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>49</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -1577,7 +1577,7 @@
         <v>54</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -1603,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -1629,7 +1629,7 @@
         <v>60</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1655,7 +1655,7 @@
         <v>62</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -1681,7 +1681,7 @@
         <v>5</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1707,7 +1707,7 @@
         <v>77</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1733,7 +1733,7 @@
         <v>81</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1759,7 +1759,7 @@
         <v>85</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1785,7 +1785,7 @@
         <v>89</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1811,7 +1811,7 @@
         <v>93</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1837,7 +1837,7 @@
         <v>97</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="91" x14ac:dyDescent="0.2">
@@ -1863,7 +1863,7 @@
         <v>54</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1889,7 +1889,7 @@
         <v>103</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -1915,7 +1915,7 @@
         <v>12</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
         <v>110</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
         <v>43</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -1993,7 +1993,7 @@
         <v>115</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2019,7 +2019,7 @@
         <v>119</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2045,7 +2045,7 @@
         <v>122</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -2071,7 +2071,7 @@
         <v>97</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -2097,7 +2097,7 @@
         <v>128</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -2123,7 +2123,7 @@
         <v>12</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -2149,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2175,7 +2175,7 @@
         <v>139</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="76" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>7</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="46" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
         <v>146</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>64</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2279,7 +2279,7 @@
         <v>24</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="31" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
         <v>156</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2357,7 +2357,7 @@
         <v>27</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2383,7 +2383,7 @@
         <v>161</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2409,7 +2409,7 @@
         <v>165</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="61" x14ac:dyDescent="0.2">
@@ -2435,7 +2435,7 @@
         <v>177</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>